<commit_message>
create enginerring department detail
</commit_message>
<xml_diff>
--- a/public/workers.xlsx
+++ b/public/workers.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Personal" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Departments" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Employees" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,33 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
   <si>
     <t>Employee_number</t>
-  </si>
-  <si>
-    <t>First_name</t>
-  </si>
-  <si>
-    <t>Second_name</t>
-  </si>
-  <si>
-    <t>Third_name</t>
-  </si>
-  <si>
-    <t>National_id</t>
-  </si>
-  <si>
-    <t>KRA_pin</t>
-  </si>
-  <si>
-    <t>NHIF_number</t>
-  </si>
-  <si>
-    <t>NSSF_number</t>
-  </si>
-  <si>
-    <t>bank_account_number</t>
   </si>
 </sst>
 </file>
@@ -87,6 +73,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -293,9 +283,31 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.0"/>
-    <col customWidth="1" min="2" max="2" width="9.38"/>
+    <col customWidth="1" min="1" max="2" width="15.0"/>
     <col customWidth="1" min="3" max="3" width="11.75"/>
     <col customWidth="1" min="4" max="4" width="9.88"/>
     <col customWidth="1" min="5" max="5" width="9.38"/>
@@ -307,31 +319,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>